<commit_message>
Rerun model 3 and model 7
</commit_message>
<xml_diff>
--- a/data/data_collection.xlsx
+++ b/data/data_collection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4620125-426F-4140-975F-5562E4F12552}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAD0CB2-755C-4A3A-8E5C-0627204B2779}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="5813" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig 3" sheetId="1" r:id="rId1"/>
@@ -6822,7 +6822,7 @@
   <dimension ref="A1:DT66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Change maximal flux value. Add all tissue running mode for all glucose and lactate infused mice in Rabinowitz's data.
</commit_message>
<xml_diff>
--- a/data/data_collection.xlsx
+++ b/data/data_collection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BD214C-D031-4327-A061-12CACA25B0EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8847588B-DEC1-41DD-96E1-BC773AF512D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="24420" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig 3" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,6 @@
     <sheet name="Sup_Fig_5_fasted_lactate" sheetId="4" r:id="rId4"/>
     <sheet name="Data figures" sheetId="5" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -9331,66 +9328,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="no_tumor_glucose"/>
-      <sheetName val="Figures"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="56">
-          <cell r="M56" t="str">
-            <v>m+0</v>
-          </cell>
-          <cell r="N56">
-            <v>0.87658399527497344</v>
-          </cell>
-          <cell r="O56">
-            <v>6.1208930391433755E-2</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="M57" t="str">
-            <v>m+1</v>
-          </cell>
-          <cell r="N57">
-            <v>1.7264258490620035E-2</v>
-          </cell>
-          <cell r="O57">
-            <v>1.4760876630039648E-2</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="M58" t="str">
-            <v>m+2</v>
-          </cell>
-          <cell r="N58">
-            <v>0</v>
-          </cell>
-          <cell r="O58">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="M59" t="str">
-            <v>m+3</v>
-          </cell>
-          <cell r="N59">
-            <v>0.10615174623440654</v>
-          </cell>
-          <cell r="O59">
-            <v>4.6870240380017421E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12241,8 +12178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91A95FF-790F-41A9-B52C-37FE637D906C}">
   <dimension ref="A1:DT66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="DF27" sqref="DF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -32348,7 +32285,7 @@
   <dimension ref="A1:CV66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25:I29"/>
+      <selection activeCell="AZ23" sqref="AZ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -49898,7 +49835,7 @@
   <dimension ref="A2:R38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>